<commit_message>
Deploying to gh-pages from  @ 6102771c89069f5ae66a23894170c82bab8b3142 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.a.1.xlsx
+++ b/en/downloads/data-excel/2.a.1.xlsx
@@ -47,9 +47,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,7 +221,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,11 +530,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -546,7 +541,7 @@
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -569,7 +564,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="5"/>
       <c r="C2" s="14"/>
@@ -586,7 +581,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -635,8 +630,11 @@
       <c r="P3" s="12">
         <v>2019</v>
       </c>
+      <c r="Q3" s="12">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -685,13 +683,16 @@
       <c r="P4" s="18">
         <v>8.1158584953197901E-2</v>
       </c>
+      <c r="Q4" s="18">
+        <v>6.7156049127444606E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ f300734639cb36e034c6627e828e5fab9702d198 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/2.a.1.xlsx
+++ b/en/downloads/data-excel/2.a.1.xlsx
@@ -47,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,6 +124,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -172,7 +178,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -222,6 +228,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -530,9 +539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,7 +552,7 @@
     <col min="3" max="3" width="37.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>8</v>
       </c>
@@ -564,7 +575,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:17" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14"/>
       <c r="B2" s="5"/>
       <c r="C2" s="14"/>
@@ -581,7 +592,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -633,8 +644,11 @@
       <c r="Q3" s="12">
         <v>2020</v>
       </c>
+      <c r="R3" s="12">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
@@ -686,13 +700,16 @@
       <c r="Q4" s="18">
         <v>6.7156049127444606E-2</v>
       </c>
+      <c r="R4" s="19">
+        <v>5.7927248158369672E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="11"/>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="11"/>
     </row>
   </sheetData>

</xml_diff>